<commit_message>
Added textbook to explain this analysis was replaced by the cross-section elevation analysis
</commit_message>
<xml_diff>
--- a/data/Excel_LO_edited/Vegetation monitoring point elevation change data_LO.xlsx
+++ b/data/Excel_LO_edited/Vegetation monitoring point elevation change data_LO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_email_arizona_edu/Documents/grad school/Gornish lab/Altar Valley Conservation Alliance Elkhorn-Las Delicias Demo/AVCA_ElkLD/data/Excel_LO_edited/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/02_AVCA Elkhorn-Las Delicias/AVCA_ElkLD/data/Excel_LO_edited/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{80399F5D-E855-4D12-9D5F-4046741A505B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8833EEA-D773-466F-877B-B7399560638C}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{80399F5D-E855-4D12-9D5F-4046741A505B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57CDB50E-C89C-4E0F-AA67-BA51525DB1D5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vegetation monitoring point ele" sheetId="1" r:id="rId1"/>
@@ -967,6 +967,95 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FA5B341-B42E-6403-EC7E-8BA6406F6E80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3032760" y="381000"/>
+          <a:ext cx="4000500" cy="1341120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Initial analysis</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> from Robert Davis.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Has since been replaced with more comprehensive analysis of entire cross section of elevation change that we hired him to do</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1268,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1972,6 +2061,7 @@
     <sortCondition ref="A1:A63"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1979,7 +2069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6ECC86E-BC94-4D49-87FF-441231CA3CC2}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>

</xml_diff>